<commit_message>
modified:   .gitignore 	modified:   Problem_data.xlsx 	modified:   src/greedy_Q.py
</commit_message>
<xml_diff>
--- a/Problem_data.xlsx
+++ b/Problem_data.xlsx
@@ -483,10 +483,10 @@
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>1355</v>
+        <v>1358</v>
       </c>
       <c r="F2" t="n">
-        <v>735</v>
+        <v>737</v>
       </c>
     </row>
     <row r="3">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1629</v>
+        <v>1634</v>
       </c>
       <c r="F3" t="n">
         <v>255</v>
@@ -539,10 +539,10 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="F4" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5">
@@ -567,10 +567,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F5" t="n">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6">
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -727,10 +727,10 @@
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="F11" t="n">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12">
@@ -775,10 +775,10 @@
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="F13" t="n">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14">
@@ -799,7 +799,7 @@
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F14" t="n">
         <v>119</v>
@@ -919,10 +919,10 @@
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F19" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20">
@@ -1751,10 +1751,10 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F50" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">

</xml_diff>